<commit_message>
updated Tmp folder with older results in form of pdfs
</commit_message>
<xml_diff>
--- a/Tmp/languages_germany_crs.xlsx
+++ b/Tmp/languages_germany_crs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7152"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
   <si>
     <t>language</t>
   </si>
@@ -187,18 +187,6 @@
   </si>
   <si>
     <t>percent</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
   <si>
     <t>difference</t>
@@ -3515,22 +3503,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" zoomScale="81" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="52.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="33.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="52.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="9" max="9" width="33.88671875" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3547,19 +3535,19 @@
         <v>54</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3582,7 +3570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3607,7 +3595,7 @@
         <v>0.17832653232930881</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -3638,7 +3626,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3663,7 +3651,7 @@
         <v>6.7140633545075934E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -3674,7 +3662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3685,7 +3673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -3702,19 +3690,19 @@
         <v>54</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -3737,7 +3725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -3762,7 +3750,7 @@
         <v>5.7131912720256507E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3793,7 +3781,7 @@
         <v>6219</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -3817,8 +3805,12 @@
         <f t="shared" si="3"/>
         <v>0.22262576965638567</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <f xml:space="preserve"> 237*100/68</f>
+        <v>348.52941176470586</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -3829,7 +3821,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -3840,7 +3832,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -3851,19 +3843,19 @@
         <v>514</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -3886,7 +3878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -3911,7 +3903,7 @@
         <v>0.13969550272356784</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -3936,7 +3928,7 @@
         <v>0.11513155271280116</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -3961,7 +3953,7 @@
         <v>0.6614800577412332</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -3972,7 +3964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -3983,7 +3975,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -3994,7 +3986,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -4005,7 +3997,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -4016,7 +4008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -4027,7 +4019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -4038,7 +4030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -4049,7 +4041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -4060,7 +4052,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -4071,7 +4063,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -4082,7 +4074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -4093,7 +4085,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -4104,7 +4096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -4115,7 +4107,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -4126,7 +4118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -4137,7 +4129,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -4148,7 +4140,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -4159,7 +4151,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -4170,7 +4162,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -4181,7 +4173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -4192,7 +4184,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -4203,7 +4195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -4214,7 +4206,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -4225,7 +4217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -4236,7 +4228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -4247,7 +4239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>47</v>
       </c>

</xml_diff>